<commit_message>
With underlay and pdf
</commit_message>
<xml_diff>
--- a/heroes.xlsx
+++ b/heroes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>(-) The team doesn't knows how</t>
   </si>
   <si>
-    <t>Avatar</t>
-  </si>
-  <si>
     <t xml:space="preserve">CCSar </t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>(-) The team doesn't learn from errors</t>
   </si>
   <si>
-    <t>CaptainDelegate *</t>
-  </si>
-  <si>
     <t>(+) He can bring any team to self-organize</t>
   </si>
   <si>
@@ -91,9 +85,6 @@
     <t>&lt;+&gt; used with restrain is good, but if used too extensively, it leads to &lt;-&gt;</t>
   </si>
   <si>
-    <t>SolveZero *</t>
-  </si>
-  <si>
     <t xml:space="preserve">(+) He can motivate anyone to solve their own problems </t>
   </si>
   <si>
@@ -223,9 +214,6 @@
     <t>(+) Relies purely and extensively on metrics, no more guts Feelings</t>
   </si>
   <si>
-    <t>(-) "If you give a manager a target, he will meet it, even if he has to destroy the organization to do so." (Demming)</t>
-  </si>
-  <si>
     <t>Perfectionist</t>
   </si>
   <si>
@@ -253,40 +241,64 @@
     <t>Background</t>
   </si>
   <si>
-    <t>svg/1.svg</t>
-  </si>
-  <si>
-    <t>svg/2.svg</t>
-  </si>
-  <si>
-    <t>svg/3.svg</t>
-  </si>
-  <si>
-    <t>svg/4.svg</t>
-  </si>
-  <si>
-    <t>svg/5.svg</t>
-  </si>
-  <si>
-    <t>svg/6.svg</t>
-  </si>
-  <si>
-    <t>svg/green.svg</t>
-  </si>
-  <si>
-    <t>svg/brown.svg</t>
-  </si>
-  <si>
-    <t>svg/dark_grey.svg</t>
-  </si>
-  <si>
-    <t>svg/white.svg</t>
-  </si>
-  <si>
-    <t>svg/yellow.svg</t>
-  </si>
-  <si>
-    <t>svg/orange.svg</t>
+    <t>svg/a.svg</t>
+  </si>
+  <si>
+    <t>svg/b.svg</t>
+  </si>
+  <si>
+    <t>svg/c.svg</t>
+  </si>
+  <si>
+    <t>svg/d.svg</t>
+  </si>
+  <si>
+    <t>svg/e.svg</t>
+  </si>
+  <si>
+    <t>svg/f.svg</t>
+  </si>
+  <si>
+    <t>svg/g.svg</t>
+  </si>
+  <si>
+    <t>svg/h.svg</t>
+  </si>
+  <si>
+    <t>svg/i.svg</t>
+  </si>
+  <si>
+    <t>svg/j.svg</t>
+  </si>
+  <si>
+    <t>svg/k.svg</t>
+  </si>
+  <si>
+    <t>svg/l.svg</t>
+  </si>
+  <si>
+    <t>svg/m.svg</t>
+  </si>
+  <si>
+    <t>svg/n.svg</t>
+  </si>
+  <si>
+    <t>svg/o.svg</t>
+  </si>
+  <si>
+    <t>svg/p.svg</t>
+  </si>
+  <si>
+    <t>svg/q.svg</t>
+  </si>
+  <si>
+    <t>(-) If you give a manager a target, he will meet it, even if he has to destroy the organization to do so</t>
+  </si>
+  <si>
+    <t>CaptainDelegate</t>
+  </si>
+  <si>
+    <t>SolveZero</t>
   </si>
 </sst>
 </file>
@@ -646,22 +658,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:E19"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,13 +683,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -689,13 +697,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -706,265 +711,217 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>78</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
         <v>70</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C18" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" t="s">
-        <v>75</v>
-      </c>
       <c r="D18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -984,93 +941,93 @@
   <sheetData>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B61" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C61" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B62" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C62" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C64" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed FifthWhy to have only 16
</commit_message>
<xml_diff>
--- a/heroes.xlsx
+++ b/heroes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -166,9 +166,6 @@
     <t>svg/k.svg</t>
   </si>
   <si>
-    <t>svg/l.svg</t>
-  </si>
-  <si>
     <t>svg/m.svg</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>when the house is burning you sometimes do need answers</t>
   </si>
   <si>
-    <t>efficiency and self-ownership tend to go down the drain</t>
-  </si>
-  <si>
     <t>But</t>
   </si>
   <si>
@@ -287,12 +281,6 @@
   </si>
   <si>
     <t>the team is all-in and failures are extremely painful</t>
-  </si>
-  <si>
-    <t>She can make anyone search for the deepest "why"</t>
-  </si>
-  <si>
-    <t>Fifthswhy</t>
   </si>
   <si>
     <t>Voices of the oppressed, he makes sure everyone gets heard</t>
@@ -387,8 +375,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:E23" totalsRowShown="0">
-  <autoFilter ref="A1:E23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:E22" totalsRowShown="0">
+  <autoFilter ref="A1:E22"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Plus"/>
@@ -697,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -720,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -734,13 +722,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>45</v>
@@ -751,13 +739,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
@@ -768,13 +756,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
         <v>39</v>
@@ -785,13 +773,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
         <v>40</v>
@@ -802,13 +790,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
@@ -816,16 +804,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
         <v>42</v>
@@ -833,16 +821,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
@@ -853,16 +841,16 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -870,16 +858,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -887,13 +875,13 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
         <v>46</v>
@@ -904,13 +892,13 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
@@ -918,16 +906,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
         <v>48</v>
@@ -935,110 +923,110 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D15" t="s">
-        <v>94</v>
-      </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" t="s">
-        <v>95</v>
-      </c>
       <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>97</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
         <v>76</v>
@@ -1046,53 +1034,36 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Two more empty superheroes
</commit_message>
<xml_diff>
--- a/heroes.xlsx
+++ b/heroes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -311,6 +311,15 @@
   </si>
   <si>
     <t>the atmosphere becomes dull as members turn robot-like</t>
+  </si>
+  <si>
+    <t>svg/l.svg</t>
+  </si>
+  <si>
+    <t>svg/w.svg</t>
+  </si>
+  <si>
+    <t>svg/x.svg</t>
   </si>
 </sst>
 </file>
@@ -375,8 +384,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:E22" totalsRowShown="0">
-  <autoFilter ref="A1:E22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:E25" totalsRowShown="0">
+  <autoFilter ref="A1:E25"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Plus"/>
@@ -685,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1064,6 +1073,39 @@
       </c>
       <c r="E22" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update post oliver Review
</commit_message>
<xml_diff>
--- a/heroes.xlsx
+++ b/heroes.xlsx
@@ -184,9 +184,6 @@
     <t>CaptainDelegate</t>
   </si>
   <si>
-    <t>SolveZero</t>
-  </si>
-  <si>
     <t xml:space="preserve">She can manage 1000 tasks in parallel </t>
   </si>
   <si>
@@ -199,15 +196,6 @@
     <t xml:space="preserve">He can make any conflict disappear </t>
   </si>
   <si>
-    <t xml:space="preserve">She never makes any mistake, never takes any risk </t>
-  </si>
-  <si>
-    <t>He can bring any team to self-organize</t>
-  </si>
-  <si>
-    <t>His team is very well informed of what is happening around them</t>
-  </si>
-  <si>
     <t xml:space="preserve">Anyone feels super safe to openly talk about their problems </t>
   </si>
   <si>
@@ -259,12 +247,6 @@
     <t>svg/v.svg</t>
   </si>
   <si>
-    <t xml:space="preserve">She can motivate anyone to solve their own problems </t>
-  </si>
-  <si>
-    <t>when the house is burning you sometimes do need answers</t>
-  </si>
-  <si>
     <t>But</t>
   </si>
   <si>
@@ -277,9 +259,6 @@
     <t>encourages employees to switch off their brains</t>
   </si>
   <si>
-    <t>the team is left alone to solve those</t>
-  </si>
-  <si>
     <t>the team is all-in and failures are extremely painful</t>
   </si>
   <si>
@@ -292,9 +271,6 @@
     <t>Relies purely and extensively on metrics, no more guts feelings</t>
   </si>
   <si>
-    <t>the team will game any metric over time</t>
-  </si>
-  <si>
     <t>Reviews and corrects each team member's work</t>
   </si>
   <si>
@@ -307,9 +283,6 @@
     <t>iRobot</t>
   </si>
   <si>
-    <t>Never shows any emotions</t>
-  </si>
-  <si>
     <t>the atmosphere becomes dull as members turn robot-like</t>
   </si>
   <si>
@@ -320,6 +293,33 @@
   </si>
   <si>
     <t>svg/x.svg</t>
+  </si>
+  <si>
+    <t>FifthWhy</t>
+  </si>
+  <si>
+    <t>She can make anyone search for the deepest "why"</t>
+  </si>
+  <si>
+    <t>the team loses efficiency and commitment tends to go down the drain</t>
+  </si>
+  <si>
+    <t>She never makes any mistake</t>
+  </si>
+  <si>
+    <t>He delegates everything &amp; always at the right person</t>
+  </si>
+  <si>
+    <t>Everything he does is perfectly and extensively documented</t>
+  </si>
+  <si>
+    <t>but the team avoids asking when they really need help</t>
+  </si>
+  <si>
+    <t>emotions are ignored and metrics get gamed</t>
+  </si>
+  <si>
+    <t>Removes emotion from every discussion</t>
   </si>
 </sst>
 </file>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -717,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -731,13 +731,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>45</v>
@@ -748,13 +748,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
@@ -765,13 +765,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
         <v>39</v>
@@ -782,13 +782,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
         <v>40</v>
@@ -799,13 +799,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
@@ -816,13 +816,13 @@
         <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
         <v>42</v>
@@ -830,16 +830,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
@@ -850,13 +850,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
         <v>50</v>
@@ -867,13 +867,13 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
         <v>49</v>
@@ -884,13 +884,13 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
         <v>46</v>
@@ -901,13 +901,13 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
@@ -918,13 +918,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E13" t="s">
         <v>48</v>
@@ -935,13 +935,13 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E14" t="s">
         <v>43</v>
@@ -952,13 +952,13 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E15" t="s">
         <v>51</v>
@@ -966,41 +966,41 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" t="s">
@@ -1009,50 +1009,50 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
         <v>52</v>
@@ -1060,52 +1060,52 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove double 'but' from superpowers
</commit_message>
<xml_diff>
--- a/heroes.xlsx
+++ b/heroes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tim\Documents\Amazing.Repos\AgileSuperheroes CardGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpfeuffe\Downloads\AgileLeagueOfShortsightedSuperheroes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Tabelle1" sheetId="5" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" calcMode="autoNoTable"/>
 </workbook>
 </file>
 
@@ -304,9 +304,6 @@
     <t>Everything he does is perfectly and extensively documented</t>
   </si>
   <si>
-    <t>but the team avoids asking when they really need help</t>
-  </si>
-  <si>
     <t>emotions are ignored and metrics get gamed</t>
   </si>
   <si>
@@ -320,12 +317,15 @@
   </si>
   <si>
     <t>Delegata</t>
+  </si>
+  <si>
+    <t>the team avoids asking when they really need help</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -367,8 +367,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Erklärender Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -697,19 +697,19 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" customWidth="1"/>
-    <col min="4" max="4" width="62.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -726,7 +726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -743,7 +743,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -754,13 +754,13 @@
         <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -777,7 +777,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -794,7 +794,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -811,12 +811,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
         <v>74</v>
@@ -828,7 +828,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -845,7 +845,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -862,7 +862,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -879,7 +879,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -896,7 +896,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -907,13 +907,13 @@
         <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -930,7 +930,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -941,13 +941,13 @@
         <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -964,12 +964,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
         <v>74</v>
@@ -981,7 +981,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -998,7 +998,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>74</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>74</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>74</v>
       </c>
@@ -1125,19 +1125,19 @@
       <selection activeCell="A91" sqref="A91:C95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>23</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>29</v>
       </c>
@@ -1203,17 +1203,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>34</v>
       </c>

</xml_diff>